<commit_message>
Implement boundaries, update vignette and purpose.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/purpose.xlsx
+++ b/inst/extdata/purpose.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
@@ -17,16 +17,18 @@
     <sheet name="SSW ENE" sheetId="8" r:id="rId8"/>
     <sheet name="ABOVE LEFT" sheetId="10" r:id="rId9"/>
     <sheet name="BELOW RIGHT" sheetId="11" r:id="rId10"/>
+    <sheet name="ABOVE LEFT border" sheetId="15" r:id="rId11"/>
+    <sheet name="BELOW RIGHT border" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="32">
   <si>
     <t>Sex</t>
   </si>
@@ -911,6 +913,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="19" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -928,9 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1676,7 +1678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:H15" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2076,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2084,7 +2086,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="25" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2366,6 +2368,569 @@
       <c r="H15" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="I15" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7000</v>
+      </c>
+      <c r="E4" s="9">
+        <v>12000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>27000</v>
+      </c>
+      <c r="H4" s="9">
+        <v>137000</v>
+      </c>
+      <c r="I4" s="4">
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>29000</v>
+      </c>
+      <c r="E5" s="10">
+        <v>34000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>30000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>161000</v>
+      </c>
+      <c r="H5" s="10">
+        <v>179000</v>
+      </c>
+      <c r="I5" s="6">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="10">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>14000</v>
+      </c>
+      <c r="H6" s="10">
+        <v>66000</v>
+      </c>
+      <c r="I6" s="6">
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="10">
+        <v>11000</v>
+      </c>
+      <c r="F7" s="6">
+        <v>19000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43000</v>
+      </c>
+      <c r="H7" s="10">
+        <v>36000</v>
+      </c>
+      <c r="I7" s="6">
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="11">
+        <v>5000</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6000</v>
+      </c>
+      <c r="G8" s="7">
+        <v>6000</v>
+      </c>
+      <c r="H8" s="11">
+        <v>86000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="9">
+        <v>9000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13000</v>
+      </c>
+      <c r="H9" s="9">
+        <v>81000</v>
+      </c>
+      <c r="I9" s="4">
+        <v>66000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>30000</v>
+      </c>
+      <c r="E10" s="10">
+        <v>31000</v>
+      </c>
+      <c r="F10" s="6">
+        <v>23000</v>
+      </c>
+      <c r="G10" s="5">
+        <v>190000</v>
+      </c>
+      <c r="H10" s="10">
+        <v>219000</v>
+      </c>
+      <c r="I10" s="6">
+        <v>199000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9000</v>
+      </c>
+      <c r="E11" s="10">
+        <v>8000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="5">
+        <v>11000</v>
+      </c>
+      <c r="H11" s="10">
+        <v>47000</v>
+      </c>
+      <c r="I11" s="6">
+        <v>58000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="10">
+        <v>21000</v>
+      </c>
+      <c r="F12" s="6">
+        <v>17000</v>
+      </c>
+      <c r="G12" s="5">
+        <v>37000</v>
+      </c>
+      <c r="H12" s="10">
+        <v>50000</v>
+      </c>
+      <c r="I12" s="6">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="11">
+        <v>7000</v>
+      </c>
+      <c r="F13" s="8">
+        <v>6000</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="11">
+        <v>60000</v>
+      </c>
+      <c r="I13" s="8">
+        <v>68000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <v>7000</v>
+      </c>
+      <c r="E4" s="9">
+        <v>12000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>27000</v>
+      </c>
+      <c r="H4" s="9">
+        <v>137000</v>
+      </c>
+      <c r="I4" s="4">
+        <v>64000</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="5">
+        <v>29000</v>
+      </c>
+      <c r="E5" s="10">
+        <v>34000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>30000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>161000</v>
+      </c>
+      <c r="H5" s="10">
+        <v>179000</v>
+      </c>
+      <c r="I5" s="6">
+        <v>210000</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+      <c r="E6" s="10">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>14000</v>
+      </c>
+      <c r="H6" s="10">
+        <v>66000</v>
+      </c>
+      <c r="I6" s="6">
+        <v>68000</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="10">
+        <v>11000</v>
+      </c>
+      <c r="F7" s="6">
+        <v>19000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43000</v>
+      </c>
+      <c r="H7" s="10">
+        <v>36000</v>
+      </c>
+      <c r="I7" s="6">
+        <v>91000</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="7"/>
+      <c r="E8" s="11">
+        <v>5000</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6000</v>
+      </c>
+      <c r="G8" s="7">
+        <v>6000</v>
+      </c>
+      <c r="H8" s="11">
+        <v>86000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>55000</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="9">
+        <v>9000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13000</v>
+      </c>
+      <c r="H9" s="9">
+        <v>81000</v>
+      </c>
+      <c r="I9" s="4">
+        <v>66000</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="5">
+        <v>30000</v>
+      </c>
+      <c r="E10" s="10">
+        <v>31000</v>
+      </c>
+      <c r="F10" s="6">
+        <v>23000</v>
+      </c>
+      <c r="G10" s="5">
+        <v>190000</v>
+      </c>
+      <c r="H10" s="10">
+        <v>219000</v>
+      </c>
+      <c r="I10" s="6">
+        <v>199000</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="5">
+        <v>9000</v>
+      </c>
+      <c r="E11" s="10">
+        <v>8000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="5">
+        <v>11000</v>
+      </c>
+      <c r="H11" s="10">
+        <v>47000</v>
+      </c>
+      <c r="I11" s="6">
+        <v>58000</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="10">
+        <v>21000</v>
+      </c>
+      <c r="F12" s="6">
+        <v>17000</v>
+      </c>
+      <c r="G12" s="5">
+        <v>37000</v>
+      </c>
+      <c r="H12" s="10">
+        <v>50000</v>
+      </c>
+      <c r="I12" s="6">
+        <v>75000</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="7"/>
+      <c r="E13" s="11">
+        <v>7000</v>
+      </c>
+      <c r="F13" s="8">
+        <v>6000</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="11">
+        <v>60000</v>
+      </c>
+      <c r="I13" s="8">
+        <v>68000</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="7"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="8"/>
     </row>
   </sheetData>
@@ -2415,12 +2980,12 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
@@ -2449,10 +3014,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -2469,8 +3034,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
@@ -2485,8 +3050,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
       </c>
@@ -2501,8 +3066,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
@@ -2517,8 +3082,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="19" t="s">
         <v>15</v>
       </c>
@@ -2533,8 +3098,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2551,8 +3116,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
@@ -2567,8 +3132,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
@@ -2583,8 +3148,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -2599,8 +3164,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
@@ -2615,8 +3180,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -2633,8 +3198,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
@@ -2649,8 +3214,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
@@ -2665,8 +3230,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="19" t="s">
         <v>13</v>
       </c>
@@ -2681,8 +3246,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
@@ -2697,8 +3262,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -2715,8 +3280,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="19" t="s">
         <v>10</v>
       </c>
@@ -2731,8 +3296,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="19" t="s">
         <v>11</v>
       </c>
@@ -2747,8 +3312,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="19" t="s">
         <v>13</v>
       </c>
@@ -2763,8 +3328,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="19" t="s">
         <v>15</v>
       </c>
@@ -2779,10 +3344,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -2799,8 +3364,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="19" t="s">
         <v>10</v>
       </c>
@@ -2815,8 +3380,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="19" t="s">
         <v>11</v>
       </c>
@@ -2831,8 +3396,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="19" t="s">
         <v>13</v>
       </c>
@@ -2847,8 +3412,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="19" t="s">
         <v>15</v>
       </c>
@@ -2863,8 +3428,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="28" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -2881,8 +3446,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="19" t="s">
         <v>10</v>
       </c>
@@ -2897,8 +3462,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="19" t="s">
         <v>11</v>
       </c>
@@ -2913,8 +3478,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="19" t="s">
         <v>13</v>
       </c>
@@ -2929,8 +3494,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="19" t="s">
         <v>15</v>
       </c>
@@ -2945,8 +3510,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="30"/>
+      <c r="B35" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -2963,8 +3528,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="19" t="s">
         <v>10</v>
       </c>
@@ -2979,8 +3544,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="19" t="s">
         <v>11</v>
       </c>
@@ -2995,8 +3560,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="19" t="s">
         <v>13</v>
       </c>
@@ -3011,8 +3576,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="19" t="s">
         <v>15</v>
       </c>
@@ -3027,8 +3592,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="28" t="s">
+      <c r="A40" s="30"/>
+      <c r="B40" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="19" t="s">
@@ -3045,8 +3610,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="19" t="s">
         <v>10</v>
       </c>
@@ -3061,8 +3626,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="19" t="s">
         <v>11</v>
       </c>
@@ -3077,8 +3642,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="19" t="s">
         <v>13</v>
       </c>
@@ -3093,8 +3658,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="19" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Rework and document 'purpose' dataset
</commit_message>
<xml_diff>
--- a/inst/extdata/purpose.xlsx
+++ b/inst/extdata/purpose.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
@@ -22,13 +22,13 @@
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="42">
   <si>
     <t>Sex</t>
   </si>
@@ -124,6 +124,36 @@
   </si>
   <si>
     <t>The data is 'Sense of purpose by highest qualification, age group, and sex, 2014' from the Statistics New Zealand portal [NZ.Stat](http://nzdotstat.stats.govt.nz/wbos/Index.aspx#), retrieved on 2016-08-19.</t>
+  </si>
+  <si>
+    <t>It can be found in the section 'People and communities' &gt; 'Self-rated well-being (NZGSS)'.</t>
+  </si>
+  <si>
+    <t>The description provided by Statistics New Zealand is below.</t>
+  </si>
+  <si>
+    <t>The 2014 New Zealand General Social Survey (NZGSS) is the fourth of the survey series. We run the NZGSS every two years and interview around 8,500 people about a range of social and economic outcomes.</t>
+  </si>
+  <si>
+    <t>Symbols used in this table:</t>
+  </si>
+  <si>
+    <t>S - Data has been suppressed.</t>
+  </si>
+  <si>
+    <t>* - Relative sampling error of 50 percent or more. Numbers may not add to the total because 'Don't know' and 'Refused' have been excluded.</t>
+  </si>
+  <si>
+    <t>For more tables using the NZGSS 2014 first release see here.</t>
+  </si>
+  <si>
+    <t>Data quality</t>
+  </si>
+  <si>
+    <t>These statistics have been produced in accordance with the Official Statistics System principles and protocols for quality. They conform to the Statistics NZ Methodological Standard for Reporting of Data Quality.</t>
+  </si>
+  <si>
+    <t>It provides new and redeveloped data about different aspects of people's lives and their well-being. In particular, the survey provides a view of how well-being outcomes are distributed across different groups within the New Zealand population.</t>
   </si>
 </sst>
 </file>
@@ -916,6 +946,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="24" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="19" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -924,15 +963,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="20" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="24" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1678,7 +1708,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:H15" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2076,9 +2106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2088,6 +2120,56 @@
     <row r="1" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2379,7 +2461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2980,12 +3062,12 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
@@ -3014,10 +3096,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -3034,8 +3116,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
@@ -3050,8 +3132,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
       </c>
@@ -3066,8 +3148,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
@@ -3082,8 +3164,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="19" t="s">
         <v>15</v>
       </c>
@@ -3098,8 +3180,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -3116,8 +3198,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
@@ -3132,8 +3214,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
@@ -3148,8 +3230,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -3164,8 +3246,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
@@ -3180,8 +3262,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -3198,8 +3280,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
@@ -3214,8 +3296,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
@@ -3230,8 +3312,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="19" t="s">
         <v>13</v>
       </c>
@@ -3246,8 +3328,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
@@ -3262,8 +3344,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -3280,8 +3362,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="19" t="s">
         <v>10</v>
       </c>
@@ -3296,8 +3378,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="19" t="s">
         <v>11</v>
       </c>
@@ -3312,8 +3394,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="19" t="s">
         <v>13</v>
       </c>
@@ -3328,8 +3410,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="19" t="s">
         <v>15</v>
       </c>
@@ -3344,10 +3426,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -3364,8 +3446,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="19" t="s">
         <v>10</v>
       </c>
@@ -3380,8 +3462,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="19" t="s">
         <v>11</v>
       </c>
@@ -3396,8 +3478,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="19" t="s">
         <v>13</v>
       </c>
@@ -3412,8 +3494,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="19" t="s">
         <v>15</v>
       </c>
@@ -3428,8 +3510,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="29" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -3446,8 +3528,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="19" t="s">
         <v>10</v>
       </c>
@@ -3462,8 +3544,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="19" t="s">
         <v>11</v>
       </c>
@@ -3478,8 +3560,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="19" t="s">
         <v>13</v>
       </c>
@@ -3494,8 +3576,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="19" t="s">
         <v>15</v>
       </c>
@@ -3510,8 +3592,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="29" t="s">
+      <c r="A35" s="27"/>
+      <c r="B35" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -3528,8 +3610,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="19" t="s">
         <v>10</v>
       </c>
@@ -3544,8 +3626,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="19" t="s">
         <v>11</v>
       </c>
@@ -3560,8 +3642,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="19" t="s">
         <v>13</v>
       </c>
@@ -3576,8 +3658,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="19" t="s">
         <v>15</v>
       </c>
@@ -3592,8 +3674,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="29" t="s">
+      <c r="A40" s="27"/>
+      <c r="B40" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="19" t="s">
@@ -3610,8 +3692,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="19" t="s">
         <v>10</v>
       </c>
@@ -3626,8 +3708,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="19" t="s">
         <v>11</v>
       </c>
@@ -3642,8 +3724,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="19" t="s">
         <v>13</v>
       </c>
@@ -3658,8 +3740,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="19" t="s">
         <v>15</v>
       </c>
@@ -3719,17 +3801,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A25:A44"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B40:B44"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A5:A24"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A25:A44"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B40:B44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" tooltip="Click once to display linked information. Click and hold to select this cell." display="http://nzdotstat.stats.govt.nz/OECDStat_Metadata/ShowMetadata.ashx?Dataset=TABLECODE7965&amp;ShowOnWeb=true&amp;Lang=en"/>
@@ -3747,7 +3829,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5469,7 +5551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Add partition() for small multiples
Add a sheet to partition.xlsx for examples
</commit_message>
<xml_diff>
--- a/inst/extdata/purpose.xlsx
+++ b/inst/extdata/purpose.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
@@ -19,16 +19,17 @@
     <sheet name="BELOW RIGHT" sheetId="11" r:id="rId10"/>
     <sheet name="ABOVE LEFT border" sheetId="15" r:id="rId11"/>
     <sheet name="BELOW RIGHT border" sheetId="16" r:id="rId12"/>
+    <sheet name="Small multiples" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId14"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="42">
   <si>
     <t>Sex</t>
   </si>
@@ -160,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +359,14 @@
       <color indexed="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="37">
@@ -895,7 +904,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -946,6 +955,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2106,6 +2117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2114,7 +2126,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="1" max="1" width="76.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2180,6 +2192,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="D4:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2459,6 +2472,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2741,6 +2755,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="D4:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3020,8 +3035,166 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="D1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>171000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>159000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>210000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>732000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>173000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>807000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>344000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>287000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -3030,8 +3203,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" customWidth="1"/>
+    <col min="1" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3062,12 +3235,12 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
@@ -3096,10 +3269,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -3116,8 +3289,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
@@ -3132,8 +3305,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
       </c>
@@ -3148,8 +3321,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
@@ -3164,8 +3337,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="19" t="s">
         <v>15</v>
       </c>
@@ -3180,8 +3353,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -3198,8 +3371,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
@@ -3214,8 +3387,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
@@ -3230,8 +3403,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -3246,8 +3419,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
@@ -3262,8 +3435,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -3280,8 +3453,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
@@ -3296,8 +3469,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
@@ -3312,8 +3485,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="19" t="s">
         <v>13</v>
       </c>
@@ -3328,8 +3501,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
@@ -3344,8 +3517,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -3362,8 +3535,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="19" t="s">
         <v>10</v>
       </c>
@@ -3378,8 +3551,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="19" t="s">
         <v>11</v>
       </c>
@@ -3394,8 +3567,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="19" t="s">
         <v>13</v>
       </c>
@@ -3410,8 +3583,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="19" t="s">
         <v>15</v>
       </c>
@@ -3426,10 +3599,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -3446,8 +3619,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="19" t="s">
         <v>10</v>
       </c>
@@ -3462,8 +3635,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="19" t="s">
         <v>11</v>
       </c>
@@ -3478,8 +3651,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="19" t="s">
         <v>13</v>
       </c>
@@ -3494,8 +3667,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="19" t="s">
         <v>15</v>
       </c>
@@ -3510,8 +3683,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -3528,8 +3701,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="19" t="s">
         <v>10</v>
       </c>
@@ -3544,8 +3717,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="19" t="s">
         <v>11</v>
       </c>
@@ -3560,8 +3733,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="19" t="s">
         <v>13</v>
       </c>
@@ -3576,8 +3749,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="19" t="s">
         <v>15</v>
       </c>
@@ -3592,8 +3765,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="26" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -3610,8 +3783,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="19" t="s">
         <v>10</v>
       </c>
@@ -3626,8 +3799,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="19" t="s">
         <v>11</v>
       </c>
@@ -3642,8 +3815,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="19" t="s">
         <v>13</v>
       </c>
@@ -3658,8 +3831,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="19" t="s">
         <v>15</v>
       </c>
@@ -3674,8 +3847,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="26" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="19" t="s">
@@ -3692,8 +3865,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="19" t="s">
         <v>10</v>
       </c>
@@ -3708,8 +3881,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="19" t="s">
         <v>11</v>
       </c>
@@ -3724,8 +3897,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="19" t="s">
         <v>13</v>
       </c>
@@ -3740,8 +3913,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="19" t="s">
         <v>15</v>
       </c>
@@ -3826,6 +3999,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5252,23 +5426,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A3:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="24" customWidth="1"/>
     <col min="5" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.75" customWidth="1"/>
+    <col min="12" max="12" width="9.375" customWidth="1"/>
     <col min="13" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.375" customWidth="1"/>
+    <col min="17" max="17" width="7.375" customWidth="1"/>
     <col min="18" max="20" width="7" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="21" max="21" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5549,9 +5726,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5942,6 +6120,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6333,6 +6512,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="D4:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6724,6 +6904,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="D4:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7115,6 +7296,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Update documentation to new directions
</commit_message>
<xml_diff>
--- a/inst/extdata/purpose.xlsx
+++ b/inst/extdata/purpose.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28620" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
     <sheet name="NZ.Stat export" sheetId="13" r:id="rId2"/>
     <sheet name="Tidy" sheetId="12" r:id="rId3"/>
     <sheet name="Pivot" sheetId="5" r:id="rId4"/>
-    <sheet name="NNW WNW" sheetId="6" r:id="rId5"/>
-    <sheet name="NNE WSW" sheetId="9" r:id="rId6"/>
-    <sheet name="SSE ESE" sheetId="7" r:id="rId7"/>
-    <sheet name="SSW ENE" sheetId="8" r:id="rId8"/>
-    <sheet name="ABOVE LEFT" sheetId="10" r:id="rId9"/>
-    <sheet name="BELOW RIGHT" sheetId="11" r:id="rId10"/>
-    <sheet name="ABOVE LEFT border" sheetId="15" r:id="rId11"/>
-    <sheet name="BELOW RIGHT border" sheetId="16" r:id="rId12"/>
+    <sheet name="up-left left-up" sheetId="6" r:id="rId5"/>
+    <sheet name="up-right left-down" sheetId="9" r:id="rId6"/>
+    <sheet name="right-down down-right" sheetId="7" r:id="rId7"/>
+    <sheet name="right-up down-left" sheetId="8" r:id="rId8"/>
+    <sheet name="up-ish left-ish" sheetId="10" r:id="rId9"/>
+    <sheet name="right-ish down-ish" sheetId="11" r:id="rId10"/>
+    <sheet name="up-ish left-ish border" sheetId="15" r:id="rId11"/>
+    <sheet name="right-ish down-ish border" sheetId="16" r:id="rId12"/>
     <sheet name="Small multiples" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId14"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -957,6 +957,15 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="19" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="21" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="20" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -965,15 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="19" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="21" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="20" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1719,7 +1719,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:H15" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2120,9 +2120,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2475,9 +2473,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2758,9 +2754,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="D4:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3040,9 +3034,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3235,12 +3227,12 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
@@ -3269,10 +3261,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -3289,8 +3281,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
@@ -3305,8 +3297,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
       </c>
@@ -3321,8 +3313,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
@@ -3337,8 +3329,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="19" t="s">
         <v>15</v>
       </c>
@@ -3353,8 +3345,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -3371,8 +3363,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
@@ -3387,8 +3379,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
@@ -3403,8 +3395,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -3419,8 +3411,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
@@ -3435,8 +3427,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -3453,8 +3445,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
@@ -3469,8 +3461,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
@@ -3485,8 +3477,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="19" t="s">
         <v>13</v>
       </c>
@@ -3501,8 +3493,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
@@ -3517,8 +3509,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -3535,8 +3527,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="19" t="s">
         <v>10</v>
       </c>
@@ -3551,8 +3543,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="19" t="s">
         <v>11</v>
       </c>
@@ -3567,8 +3559,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="19" t="s">
         <v>13</v>
       </c>
@@ -3583,8 +3575,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="19" t="s">
         <v>15</v>
       </c>
@@ -3599,10 +3591,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -3619,8 +3611,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="19" t="s">
         <v>10</v>
       </c>
@@ -3635,8 +3627,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="19" t="s">
         <v>11</v>
       </c>
@@ -3651,8 +3643,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="19" t="s">
         <v>13</v>
       </c>
@@ -3667,8 +3659,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="19" t="s">
         <v>15</v>
       </c>
@@ -3683,8 +3675,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="28" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -3701,8 +3693,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="19" t="s">
         <v>10</v>
       </c>
@@ -3717,8 +3709,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="19" t="s">
         <v>11</v>
       </c>
@@ -3733,8 +3725,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="19" t="s">
         <v>13</v>
       </c>
@@ -3749,8 +3741,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="19" t="s">
         <v>15</v>
       </c>
@@ -3765,8 +3757,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -3783,8 +3775,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="19" t="s">
         <v>10</v>
       </c>
@@ -3799,8 +3791,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="19" t="s">
         <v>11</v>
       </c>
@@ -3815,8 +3807,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="19" t="s">
         <v>13</v>
       </c>
@@ -3831,8 +3823,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="19" t="s">
         <v>15</v>
       </c>
@@ -3847,8 +3839,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="28" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="19" t="s">
@@ -3865,8 +3857,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="19" t="s">
         <v>10</v>
       </c>
@@ -3881,8 +3873,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="19" t="s">
         <v>11</v>
       </c>
@@ -3897,8 +3889,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="19" t="s">
         <v>13</v>
       </c>
@@ -3913,8 +3905,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="19" t="s">
         <v>15</v>
       </c>
@@ -3974,17 +3966,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A25:A44"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B40:B44"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A5:A24"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A25:A44"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B40:B44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" tooltip="Click once to display linked information. Click and hold to select this cell." display="http://nzdotstat.stats.govt.nz/OECDStat_Metadata/ShowMetadata.ashx?Dataset=TABLECODE7965&amp;ShowOnWeb=true&amp;Lang=en"/>
@@ -4002,9 +3994,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5429,9 +5419,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A3:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5729,9 +5717,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>